<commit_message>
fix bugs with import package
</commit_message>
<xml_diff>
--- a/main/excel_py.xlsx
+++ b/main/excel_py.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,11 +593,11 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>тонны, грн, за транзакцию</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R2" t="n">
@@ -2816,164 +2816,6 @@
         <v>0</v>
       </c>
       <c r="S30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>30 день</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R31" t="n">
-        <v>0</v>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>31 день</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H32" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R32" t="n">
-        <v>0</v>
-      </c>
-      <c r="S32" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>